<commit_message>
Modified controller to pick the one test script
</commit_message>
<xml_diff>
--- a/SG_Mvn_Project/ExecutionController/Controller.xlsx
+++ b/SG_Mvn_Project/ExecutionController/Controller.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SG_Maven_Framework\SG_Mvn_Project\ExecutionController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalCopy\sgTest\SG_Mvn_Project\ExecutionController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2350700C-9633-4428-A4EE-0A695A4821A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26925791-A8FF-459B-BBE7-C4475F680074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -595,7 +595,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2"/>
     </row>

</xml_diff>